<commit_message>
SW Develop. RAM Memory is now indexed by  B auxiliary register. MOV A, B(data_address) and MOV B(data_address),A
</commit_message>
<xml_diff>
--- a/Documentacion/MicroInstructions_ Matrix.xlsx
+++ b/Documentacion/MicroInstructions_ Matrix.xlsx
@@ -323,12 +323,6 @@
     <t>Operand’s Data</t>
   </si>
   <si>
-    <t>A,data addr</t>
-  </si>
-  <si>
-    <t>data addr,A</t>
-  </si>
-  <si>
     <t>Bytes</t>
   </si>
   <si>
@@ -527,9 +521,6 @@
     <t>MOV Rn, k</t>
   </si>
   <si>
-    <t>SPW_EN(31)</t>
-  </si>
-  <si>
     <t>DIR {7-4}</t>
   </si>
   <si>
@@ -539,7 +530,17 @@
     <t>DIR {15-13}</t>
   </si>
   <si>
-    <t>Execution Control {31}</t>
+    <t>Execution Control {31-30}</t>
+  </si>
+  <si>
+    <t>!SPW_EN(31)
+!SPW_ALU_END(30)</t>
+  </si>
+  <si>
+    <t>A,B(data addr)</t>
+  </si>
+  <si>
+    <t>B(data addr),A</t>
   </si>
 </sst>
 </file>
@@ -1144,45 +1145,45 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1503,7 +1504,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M24" sqref="M24"/>
+      <selection pane="topRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,37 +1537,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="72"/>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
+      <c r="A2" s="69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="69"/>
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C3" s="17"/>
@@ -1611,7 +1612,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>78</v>
@@ -1626,71 +1627,71 @@
         <v>67</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="O5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V5" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="X5" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="V5" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="X5" s="28" t="s">
+      <c r="Y5" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z5" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="Y5" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z5" s="52" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA5" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="AB5" s="74"/>
+      <c r="AA5" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB5" s="71"/>
       <c r="AC5" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -1770,10 +1771,10 @@
       <c r="Z6" s="46">
         <v>0</v>
       </c>
-      <c r="AA6" s="75">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="76"/>
+      <c r="AA6" s="72">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="73"/>
       <c r="AC6" s="33">
         <v>0</v>
       </c>
@@ -1857,10 +1858,10 @@
       <c r="Z7" s="47">
         <v>0</v>
       </c>
-      <c r="AA7" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="69"/>
+      <c r="AA7" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="75"/>
       <c r="AC7" s="36">
         <v>0</v>
       </c>
@@ -1944,10 +1945,10 @@
       <c r="Z8" s="47">
         <v>0</v>
       </c>
-      <c r="AA8" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="69"/>
+      <c r="AA8" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="75"/>
       <c r="AC8" s="36">
         <v>0</v>
       </c>
@@ -2029,10 +2030,10 @@
       <c r="Z9" s="47">
         <v>0</v>
       </c>
-      <c r="AA9" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="69"/>
+      <c r="AA9" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="75"/>
       <c r="AC9" s="36">
         <v>0</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I10" s="35">
         <v>0</v>
@@ -2090,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S10" s="34">
         <v>2</v>
@@ -2116,10 +2117,10 @@
       <c r="Z10" s="47">
         <v>0</v>
       </c>
-      <c r="AA10" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="69"/>
+      <c r="AA10" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="75"/>
       <c r="AC10" s="36">
         <v>0</v>
       </c>
@@ -2203,10 +2204,10 @@
       <c r="Z11" s="47">
         <v>0</v>
       </c>
-      <c r="AA11" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="69"/>
+      <c r="AA11" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="75"/>
       <c r="AC11" s="36">
         <v>0</v>
       </c>
@@ -2290,10 +2291,10 @@
       <c r="Z12" s="47">
         <v>0</v>
       </c>
-      <c r="AA12" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="69"/>
+      <c r="AA12" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="75"/>
       <c r="AC12" s="36">
         <v>0</v>
       </c>
@@ -2377,10 +2378,10 @@
       <c r="Z13" s="47">
         <v>0</v>
       </c>
-      <c r="AA13" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="69"/>
+      <c r="AA13" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="75"/>
       <c r="AC13" s="36">
         <v>0</v>
       </c>
@@ -2464,10 +2465,10 @@
       <c r="Z14" s="47">
         <v>0</v>
       </c>
-      <c r="AA14" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="69"/>
+      <c r="AA14" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="75"/>
       <c r="AC14" s="36">
         <v>0</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G15" s="35">
         <v>0</v>
@@ -2551,10 +2552,10 @@
       <c r="Z15" s="47">
         <v>0</v>
       </c>
-      <c r="AA15" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="69"/>
+      <c r="AA15" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="75"/>
       <c r="AC15" s="36">
         <v>0</v>
       </c>
@@ -2638,10 +2639,10 @@
       <c r="Z16" s="47">
         <v>0</v>
       </c>
-      <c r="AA16" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="69"/>
+      <c r="AA16" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="75"/>
       <c r="AC16" s="36">
         <v>0</v>
       </c>
@@ -2725,10 +2726,10 @@
       <c r="Z17" s="47">
         <v>0</v>
       </c>
-      <c r="AA17" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="69"/>
+      <c r="AA17" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="75"/>
       <c r="AC17" s="36">
         <v>0</v>
       </c>
@@ -2812,10 +2813,10 @@
       <c r="Z18" s="47">
         <v>0</v>
       </c>
-      <c r="AA18" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="69"/>
+      <c r="AA18" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="75"/>
       <c r="AC18" s="36">
         <v>0</v>
       </c>
@@ -2899,10 +2900,10 @@
       <c r="Z19" s="47">
         <v>0</v>
       </c>
-      <c r="AA19" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="69"/>
+      <c r="AA19" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="75"/>
       <c r="AC19" s="36">
         <v>0</v>
       </c>
@@ -2986,10 +2987,10 @@
       <c r="Z20" s="47">
         <v>0</v>
       </c>
-      <c r="AA20" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="69"/>
+      <c r="AA20" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="75"/>
       <c r="AC20" s="36">
         <v>0</v>
       </c>
@@ -3073,10 +3074,10 @@
       <c r="Z21" s="47">
         <v>0</v>
       </c>
-      <c r="AA21" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="69"/>
+      <c r="AA21" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="75"/>
       <c r="AC21" s="36">
         <v>0</v>
       </c>
@@ -3160,10 +3161,10 @@
       <c r="Z22" s="47">
         <v>0</v>
       </c>
-      <c r="AA22" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="69"/>
+      <c r="AA22" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="75"/>
       <c r="AC22" s="36">
         <v>0</v>
       </c>
@@ -3247,10 +3248,10 @@
       <c r="Z23" s="47">
         <v>0</v>
       </c>
-      <c r="AA23" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="69"/>
+      <c r="AA23" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="75"/>
       <c r="AC23" s="36">
         <v>0</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>17</v>
@@ -3272,7 +3273,7 @@
         <v>53</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>100</v>
+        <v>171</v>
       </c>
       <c r="G24" s="35">
         <v>0</v>
@@ -3334,10 +3335,10 @@
       <c r="Z24" s="47">
         <v>0</v>
       </c>
-      <c r="AA24" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="69"/>
+      <c r="AA24" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="75"/>
       <c r="AC24" s="36">
         <v>0</v>
       </c>
@@ -3350,7 +3351,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>18</v>
@@ -3413,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Y25" s="35">
         <v>0</v>
@@ -3421,10 +3422,10 @@
       <c r="Z25" s="48">
         <v>1</v>
       </c>
-      <c r="AA25" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="69"/>
+      <c r="AA25" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="75"/>
       <c r="AC25" s="36">
         <v>0</v>
       </c>
@@ -3437,7 +3438,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>19</v>
@@ -3508,10 +3509,10 @@
       <c r="Z26" s="47">
         <v>0</v>
       </c>
-      <c r="AA26" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="69"/>
+      <c r="AA26" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="75"/>
       <c r="AC26" s="36">
         <v>0</v>
       </c>
@@ -3524,7 +3525,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>20</v>
@@ -3533,7 +3534,7 @@
         <v>56</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="G27" s="35">
         <v>0</v>
@@ -3595,10 +3596,10 @@
       <c r="Z27" s="47">
         <v>0</v>
       </c>
-      <c r="AA27" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="69"/>
+      <c r="AA27" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="75"/>
       <c r="AC27" s="36">
         <v>0</v>
       </c>
@@ -3611,7 +3612,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>21</v>
@@ -3674,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="X28" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Y28" s="38">
         <v>1</v>
@@ -3682,10 +3683,10 @@
       <c r="Z28" s="47">
         <v>0</v>
       </c>
-      <c r="AA28" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="69"/>
+      <c r="AA28" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="75"/>
       <c r="AC28" s="36">
         <v>0</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>22</v>
@@ -3707,7 +3708,7 @@
         <v>58</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G29" s="35">
         <v>0</v>
@@ -3769,10 +3770,10 @@
       <c r="Z29" s="49">
         <v>0</v>
       </c>
-      <c r="AA29" s="68">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="69"/>
+      <c r="AA29" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="75"/>
       <c r="AC29" s="36">
         <v>0</v>
       </c>
@@ -3785,7 +3786,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>23</v>
@@ -3794,7 +3795,7 @@
         <v>59</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G30" s="35">
         <v>0</v>
@@ -3856,10 +3857,10 @@
       <c r="Z30" s="49">
         <v>0</v>
       </c>
-      <c r="AA30" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB30" s="67"/>
+      <c r="AA30" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB30" s="77"/>
       <c r="AC30" s="50">
         <v>1</v>
       </c>
@@ -3872,7 +3873,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="65" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>24</v>
@@ -3881,7 +3882,7 @@
         <v>60</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G31" s="35">
         <v>0</v>
@@ -3944,10 +3945,10 @@
         <v>0</v>
       </c>
       <c r="AA31" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB31" s="50" t="s">
         <v>156</v>
-      </c>
-      <c r="AB31" s="50" t="s">
-        <v>158</v>
       </c>
       <c r="AC31" s="50">
         <v>1</v>
@@ -3961,7 +3962,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>25</v>
@@ -3970,7 +3971,7 @@
         <v>61</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G32" s="35">
         <v>0</v>
@@ -4032,10 +4033,10 @@
       <c r="Z32" s="35">
         <v>0</v>
       </c>
-      <c r="AA32" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB32" s="67"/>
+      <c r="AA32" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB32" s="77"/>
       <c r="AC32" s="36">
         <v>0</v>
       </c>
@@ -4048,7 +4049,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>26</v>
@@ -4057,7 +4058,7 @@
         <v>62</v>
       </c>
       <c r="F33" s="47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G33" s="35">
         <v>0</v>
@@ -4119,10 +4120,10 @@
       <c r="Z33" s="35">
         <v>0</v>
       </c>
-      <c r="AA33" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB33" s="67"/>
+      <c r="AA33" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB33" s="77"/>
       <c r="AC33" s="36">
         <v>0</v>
       </c>
@@ -4135,7 +4136,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="65" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>27</v>
@@ -4144,7 +4145,7 @@
         <v>63</v>
       </c>
       <c r="F34" s="47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G34" s="35">
         <v>0</v>
@@ -4206,10 +4207,10 @@
       <c r="Z34" s="39">
         <v>0</v>
       </c>
-      <c r="AA34" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB34" s="67"/>
+      <c r="AA34" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB34" s="77"/>
       <c r="AC34" s="50">
         <v>1</v>
       </c>
@@ -4249,8 +4250,8 @@
       <c r="X35" s="35"/>
       <c r="Y35" s="35"/>
       <c r="Z35" s="47"/>
-      <c r="AA35" s="68"/>
-      <c r="AB35" s="69"/>
+      <c r="AA35" s="74"/>
+      <c r="AB35" s="75"/>
       <c r="AC35" s="36"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
@@ -4288,8 +4289,8 @@
       <c r="X36" s="35"/>
       <c r="Y36" s="35"/>
       <c r="Z36" s="47"/>
-      <c r="AA36" s="68"/>
-      <c r="AB36" s="69"/>
+      <c r="AA36" s="74"/>
+      <c r="AB36" s="75"/>
       <c r="AC36" s="36"/>
     </row>
     <row r="37" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4327,8 +4328,8 @@
       <c r="X37" s="42"/>
       <c r="Y37" s="42"/>
       <c r="Z37" s="55"/>
-      <c r="AA37" s="70"/>
-      <c r="AB37" s="71"/>
+      <c r="AA37" s="78"/>
+      <c r="AB37" s="79"/>
       <c r="AC37" s="51"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -4345,45 +4346,45 @@
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M43" s="56"/>
       <c r="N43" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="O43" s="64" t="s">
         <v>127</v>
-      </c>
-      <c r="O43" s="64" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M44" s="58"/>
       <c r="N44" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O44" s="29"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M45" s="59"/>
       <c r="N45" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O45" s="29"/>
       <c r="W45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="X45">
         <v>11111</v>
       </c>
       <c r="Y45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="Z45" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="45" t="s">
         <v>73</v>
       </c>
@@ -4391,59 +4392,59 @@
         <v>36</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J46" s="16"/>
       <c r="M46" s="60"/>
       <c r="N46" s="25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O46" s="29"/>
-      <c r="S46" s="80" t="s">
-        <v>172</v>
-      </c>
-      <c r="T46" s="77"/>
-      <c r="U46" s="77"/>
-      <c r="V46" s="77"/>
+      <c r="S46" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="T46" s="66"/>
+      <c r="U46" s="66"/>
+      <c r="V46" s="66"/>
       <c r="W46" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="X46" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Z46" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G47" s="16"/>
       <c r="I47" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J47" s="16"/>
       <c r="M47" s="61"/>
       <c r="N47" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O47" s="29"/>
-      <c r="S47" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="T47" s="78"/>
-      <c r="U47" s="78"/>
-      <c r="V47" s="78"/>
+      <c r="S47" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="T47" s="67"/>
+      <c r="U47" s="67"/>
+      <c r="V47" s="67"/>
       <c r="W47" s="6" t="s">
         <v>96</v>
       </c>
@@ -4459,33 +4460,33 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D48" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>38</v>
       </c>
       <c r="M48" s="62"/>
       <c r="N48" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O48" s="29"/>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M49" s="63"/>
       <c r="N49" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="O49" s="30"/>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>35</v>
@@ -4493,7 +4494,7 @@
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>40</v>
@@ -4501,7 +4502,7 @@
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>41</v>
@@ -4509,7 +4510,7 @@
     </row>
     <row r="53" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>42</v>
@@ -4517,18 +4518,11 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A2:AC2"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AA35:AB35"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AA37:AB37"/>
     <mergeCell ref="AA28:AB28"/>
     <mergeCell ref="AA29:AB29"/>
     <mergeCell ref="AA7:AB7"/>
@@ -4545,11 +4539,18 @@
     <mergeCell ref="AA21:AB21"/>
     <mergeCell ref="AA22:AB22"/>
     <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AA35:AB35"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AA37:AB37"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="A2:AC2"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SW Develop. AND, OR and XOR now depend on both auxiliary register and not on immediate value.
</commit_message>
<xml_diff>
--- a/Documentacion/MicroInstructions_ Matrix.xlsx
+++ b/Documentacion/MicroInstructions_ Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="172">
   <si>
     <t>HEX</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>A,k,code addr</t>
-  </si>
-  <si>
-    <t>A,k</t>
   </si>
   <si>
     <t>k</t>
@@ -948,7 +945,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1140,9 +1137,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1150,6 +1144,9 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1182,9 +1179,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1504,7 +1498,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F29" sqref="F29"/>
+      <selection pane="topRight" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1532,7 @@
   <sheetData>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1612,7 +1606,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>78</v>
@@ -1627,71 +1621,71 @@
         <v>67</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="N5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="V5" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="X5" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y5" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="V5" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="X5" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y5" s="26" t="s">
-        <v>130</v>
-      </c>
       <c r="Z5" s="52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AA5" s="70" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AB5" s="71"/>
       <c r="AC5" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -2061,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I10" s="35">
         <v>0</v>
@@ -2091,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S10" s="34">
         <v>2</v>
@@ -2490,7 +2484,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G15" s="35">
         <v>0</v>
@@ -2751,7 +2745,7 @@
         <v>47</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G18" s="35">
         <v>0</v>
@@ -2784,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="34">
         <v>1</v>
@@ -2838,7 +2832,7 @@
         <v>48</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G19" s="35">
         <v>0</v>
@@ -2871,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="34">
         <v>1</v>
@@ -3012,7 +3006,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G21" s="35">
         <v>0</v>
@@ -3099,7 +3093,7 @@
         <v>51</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G22" s="35">
         <v>0</v>
@@ -3132,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" s="34">
         <v>1</v>
@@ -3177,7 +3171,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>16</v>
@@ -3264,7 +3258,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>17</v>
@@ -3273,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="35">
         <v>0</v>
@@ -3351,7 +3345,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>18</v>
@@ -3360,7 +3354,7 @@
         <v>54</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G25" s="35">
         <v>0</v>
@@ -3414,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y25" s="35">
         <v>0</v>
@@ -3438,7 +3432,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>19</v>
@@ -3447,7 +3441,7 @@
         <v>55</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G26" s="35">
         <v>0</v>
@@ -3525,7 +3519,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>20</v>
@@ -3534,7 +3528,7 @@
         <v>56</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G27" s="35">
         <v>0</v>
@@ -3612,7 +3606,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>21</v>
@@ -3621,7 +3615,7 @@
         <v>57</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G28" s="35">
         <v>0</v>
@@ -3675,7 +3669,7 @@
         <v>1</v>
       </c>
       <c r="X28" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y28" s="38">
         <v>1</v>
@@ -3699,7 +3693,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>22</v>
@@ -3708,7 +3702,7 @@
         <v>58</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G29" s="35">
         <v>0</v>
@@ -3785,8 +3779,8 @@
       <c r="B30" s="10">
         <v>2</v>
       </c>
-      <c r="C30" s="65" t="s">
-        <v>165</v>
+      <c r="C30" s="23" t="s">
+        <v>164</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>23</v>
@@ -3795,7 +3789,7 @@
         <v>59</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G30" s="35">
         <v>0</v>
@@ -3858,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="AA30" s="76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB30" s="77"/>
       <c r="AC30" s="50">
@@ -3872,8 +3866,8 @@
       <c r="B31" s="10">
         <v>2</v>
       </c>
-      <c r="C31" s="65" t="s">
-        <v>149</v>
+      <c r="C31" s="23" t="s">
+        <v>148</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>24</v>
@@ -3882,7 +3876,7 @@
         <v>60</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G31" s="35">
         <v>0</v>
@@ -3945,10 +3939,10 @@
         <v>0</v>
       </c>
       <c r="AA31" s="53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB31" s="50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AC31" s="50">
         <v>1</v>
@@ -3961,8 +3955,8 @@
       <c r="B32" s="10">
         <v>2</v>
       </c>
-      <c r="C32" s="65" t="s">
-        <v>159</v>
+      <c r="C32" s="23" t="s">
+        <v>158</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>25</v>
@@ -3971,7 +3965,7 @@
         <v>61</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G32" s="35">
         <v>0</v>
@@ -4034,7 +4028,7 @@
         <v>0</v>
       </c>
       <c r="AA32" s="76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB32" s="77"/>
       <c r="AC32" s="36">
@@ -4048,8 +4042,8 @@
       <c r="B33" s="10">
         <v>2</v>
       </c>
-      <c r="C33" s="65" t="s">
-        <v>160</v>
+      <c r="C33" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>26</v>
@@ -4058,7 +4052,7 @@
         <v>62</v>
       </c>
       <c r="F33" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G33" s="35">
         <v>0</v>
@@ -4121,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="AA33" s="76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB33" s="77"/>
       <c r="AC33" s="36">
@@ -4135,8 +4129,8 @@
       <c r="B34" s="10">
         <v>2</v>
       </c>
-      <c r="C34" s="65" t="s">
-        <v>157</v>
+      <c r="C34" s="23" t="s">
+        <v>156</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>27</v>
@@ -4145,7 +4139,7 @@
         <v>63</v>
       </c>
       <c r="F34" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G34" s="35">
         <v>0</v>
@@ -4208,7 +4202,7 @@
         <v>0</v>
       </c>
       <c r="AA34" s="76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB34" s="77"/>
       <c r="AC34" s="50">
@@ -4346,42 +4340,42 @@
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M43" s="56"/>
       <c r="N43" s="57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O43" s="64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M44" s="58"/>
       <c r="N44" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O44" s="29"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M45" s="59"/>
       <c r="N45" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O45" s="29"/>
       <c r="W45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="X45">
         <v>11111</v>
       </c>
       <c r="Y45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Z45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4392,101 +4386,101 @@
         <v>36</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J46" s="16"/>
       <c r="M46" s="60"/>
       <c r="N46" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O46" s="29"/>
-      <c r="S46" s="68" t="s">
-        <v>169</v>
-      </c>
-      <c r="T46" s="66"/>
-      <c r="U46" s="66"/>
-      <c r="V46" s="66"/>
+      <c r="S46" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="T46" s="65"/>
+      <c r="U46" s="65"/>
+      <c r="V46" s="65"/>
       <c r="W46" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X46" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y46" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Z46" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G47" s="16"/>
       <c r="I47" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J47" s="16"/>
       <c r="M47" s="61"/>
       <c r="N47" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O47" s="29"/>
-      <c r="S47" s="80" t="s">
-        <v>170</v>
-      </c>
-      <c r="T47" s="67"/>
-      <c r="U47" s="67"/>
-      <c r="V47" s="67"/>
+      <c r="S47" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="T47" s="66"/>
+      <c r="U47" s="66"/>
+      <c r="V47" s="66"/>
       <c r="W47" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="X47" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="X47" s="6" t="s">
+      <c r="Y47" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="Y47" s="6" t="s">
+      <c r="Z47" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="Z47" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D48" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>38</v>
       </c>
       <c r="M48" s="62"/>
       <c r="N48" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O48" s="29"/>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M49" s="63"/>
       <c r="N49" s="54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O49" s="30"/>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>35</v>
@@ -4494,7 +4488,7 @@
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>40</v>
@@ -4502,7 +4496,7 @@
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>41</v>
@@ -4510,7 +4504,7 @@
     </row>
     <row r="53" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>42</v>

</xml_diff>